<commit_message>
Starting of Excersie 3
</commit_message>
<xml_diff>
--- a/Data science methods/Exercise3_data.xlsx
+++ b/Data science methods/Exercise3_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spapadokonstantakis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\PycharmProjects\vu-gpa\Data science methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36FF053-A3EB-45C4-AC3A-CD07ECA06512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C611D7D5-8F2C-4A48-88C5-E25417850CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C27C5E54-D3BB-418A-93AD-4D58CD294867}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C27C5E54-D3BB-418A-93AD-4D58CD294867}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,53 +41,18 @@
     <t>BD20 algae</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">BD20 </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Camelina</t>
-    </r>
-  </si>
-  <si>
     <t>BD20 canola</t>
   </si>
   <si>
     <t>BD20 corn</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">BD20 </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Jatropha</t>
-    </r>
-  </si>
-  <si>
     <t>BD20 palm</t>
   </si>
   <si>
     <t>BD20 tallow</t>
   </si>
   <si>
-    <t>BD20 soy</t>
-  </si>
-  <si>
     <t>E10 corn A</t>
   </si>
   <si>
@@ -127,38 +92,6 @@
     <t>E10 grain sorghum</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">E10 </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Miscanthus</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">E10 </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Miscanthus*G</t>
-    </r>
-  </si>
-  <si>
     <t>E10 MSW</t>
   </si>
   <si>
@@ -228,38 +161,6 @@
     <t>E85 grain sorghum</t>
   </si>
   <si>
-    <r>
-      <t>E85</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Miscanthus</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>E85</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Miscanthus*G</t>
-    </r>
-  </si>
-  <si>
     <t>E85 MSW</t>
   </si>
   <si>
@@ -293,44 +194,12 @@
     <t>RDI algae</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">RDI </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Camelina</t>
-    </r>
-  </si>
-  <si>
     <t>RDI canola</t>
   </si>
   <si>
     <t>RDI corn</t>
   </si>
   <si>
-    <r>
-      <t>RDI </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Jatropha</t>
-    </r>
-  </si>
-  <si>
     <t>RDI palm</t>
   </si>
   <si>
@@ -340,42 +209,10 @@
     <t>RDII algae</t>
   </si>
   <si>
-    <r>
-      <t>RDII </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Camelina</t>
-    </r>
-  </si>
-  <si>
     <t>RDII canola</t>
   </si>
   <si>
     <t>RDII corn</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">RDII </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Jatropha</t>
-    </r>
   </si>
   <si>
     <t>RDII palm</t>
@@ -662,12 +499,45 @@
       <t>kg 1,4-DCE]</t>
     </r>
   </si>
+  <si>
+    <t>BD20 Camelina</t>
+  </si>
+  <si>
+    <t>BD20 Jatropha</t>
+  </si>
+  <si>
+    <t>E10 Miscanthus</t>
+  </si>
+  <si>
+    <t>E10 Miscanthus*G</t>
+  </si>
+  <si>
+    <t>E85 Miscanthus</t>
+  </si>
+  <si>
+    <t>E85 Miscanthus*G</t>
+  </si>
+  <si>
+    <t>RDI Camelina</t>
+  </si>
+  <si>
+    <t>RDI Jatropha</t>
+  </si>
+  <si>
+    <t>RDII Camelina</t>
+  </si>
+  <si>
+    <t>RDII Jatropha</t>
+  </si>
+  <si>
+    <t>BD20 soy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -676,14 +546,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -779,10 +641,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -794,16 +656,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -814,7 +676,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -830,9 +692,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -870,7 +732,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -976,7 +838,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1118,7 +980,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1128,11 +990,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122E9D76-EB91-4A73-B7B6-2ECBBBB4476A}">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="13" width="14" customWidth="1"/>
@@ -1141,79 +1003,79 @@
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1289,7 +1151,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="B6" s="5">
         <v>15.1</v>
@@ -1330,7 +1192,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="5">
         <v>15.1</v>
@@ -1371,7 +1233,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="5">
         <v>15.1</v>
@@ -1412,7 +1274,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="B9" s="5">
         <v>15.1</v>
@@ -1453,7 +1315,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="5">
         <v>15.1</v>
@@ -1494,7 +1356,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11" s="5">
         <v>15.1</v>
@@ -1535,7 +1397,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="B12" s="5">
         <v>15.1</v>
@@ -1576,7 +1438,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B13" s="5">
         <v>10.7</v>
@@ -1617,7 +1479,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B14" s="5">
         <v>10.7</v>
@@ -1658,7 +1520,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B15" s="5">
         <v>10.7</v>
@@ -1699,7 +1561,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B16" s="5">
         <v>10.7</v>
@@ -1740,7 +1602,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B17" s="5">
         <v>10.7</v>
@@ -1781,7 +1643,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B18" s="5">
         <v>10.7</v>
@@ -1822,7 +1684,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B19" s="5">
         <v>10.7</v>
@@ -1863,7 +1725,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B20" s="5">
         <v>10.7</v>
@@ -1904,7 +1766,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B21" s="5">
         <v>10.7</v>
@@ -1945,7 +1807,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B22" s="5">
         <v>10.7</v>
@@ -1986,7 +1848,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B23" s="5">
         <v>10.7</v>
@@ -2027,7 +1889,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B24" s="5">
         <v>10.7</v>
@@ -2068,7 +1930,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B25" s="5">
         <v>10.7</v>
@@ -2109,7 +1971,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="B26" s="5">
         <v>10.7</v>
@@ -2150,7 +2012,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="B27" s="5">
         <v>10.7</v>
@@ -2191,7 +2053,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B28" s="5">
         <v>10.7</v>
@@ -2232,7 +2094,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B29" s="5">
         <v>10.7</v>
@@ -2273,7 +2135,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B30" s="5">
         <v>10.7</v>
@@ -2314,7 +2176,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B31" s="5">
         <v>10.7</v>
@@ -2355,7 +2217,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B32" s="5">
         <v>10.7</v>
@@ -2396,7 +2258,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B33" s="5">
         <v>10.7</v>
@@ -2437,7 +2299,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B34" s="5">
         <v>10.7</v>
@@ -2478,7 +2340,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B35" s="5">
         <v>10.7</v>
@@ -2519,7 +2381,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B36" s="5">
         <v>10.7</v>
@@ -2560,7 +2422,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B37" s="7">
         <v>10.7</v>
@@ -2601,7 +2463,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B38" s="5">
         <v>8.6</v>
@@ -2642,7 +2504,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B39" s="5">
         <v>8.6</v>
@@ -2683,7 +2545,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B40" s="5">
         <v>8.6</v>
@@ -2724,7 +2586,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B41" s="5">
         <v>8.6</v>
@@ -2765,7 +2627,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B42" s="5">
         <v>8.6</v>
@@ -2806,7 +2668,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B43" s="5">
         <v>8.6</v>
@@ -2847,7 +2709,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B44" s="5">
         <v>8.6</v>
@@ -2888,7 +2750,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B45" s="5">
         <v>8.6</v>
@@ -2929,7 +2791,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B46" s="5">
         <v>8.6</v>
@@ -2970,7 +2832,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B47" s="5">
         <v>8.6</v>
@@ -3011,7 +2873,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B48" s="5">
         <v>8.6</v>
@@ -3052,7 +2914,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B49" s="5">
         <v>8.6</v>
@@ -3093,7 +2955,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B50" s="5">
         <v>8.6</v>
@@ -3134,7 +2996,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B51" s="5">
         <v>8.6</v>
@@ -3175,7 +3037,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="B52" s="5">
         <v>8.6</v>
@@ -3216,7 +3078,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B53" s="5">
         <v>8.6</v>
@@ -3257,7 +3119,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B54" s="5">
         <v>8.6</v>
@@ -3298,7 +3160,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B55" s="5">
         <v>8.6</v>
@@ -3339,7 +3201,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B56" s="5">
         <v>8.6</v>
@@ -3380,7 +3242,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B57" s="5">
         <v>8.6</v>
@@ -3421,7 +3283,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B58" s="5">
         <v>8.6</v>
@@ -3462,7 +3324,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B59" s="5">
         <v>8.6</v>
@@ -3503,7 +3365,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B60" s="5">
         <v>8.6</v>
@@ -3544,7 +3406,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B61" s="5">
         <v>8.6</v>
@@ -3585,7 +3447,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B62" s="5">
         <v>8.6</v>
@@ -3626,7 +3488,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B63" s="5">
         <v>14.6</v>
@@ -3667,7 +3529,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="B64" s="5">
         <v>14.6</v>
@@ -3708,7 +3570,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B65" s="5">
         <v>14.6</v>
@@ -3749,7 +3611,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B66" s="5">
         <v>14.6</v>
@@ -3790,7 +3652,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B67" s="5">
         <v>14.6</v>
@@ -3831,7 +3693,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B68" s="5">
         <v>14.6</v>
@@ -3872,7 +3734,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B69" s="5">
         <v>14.6</v>
@@ -3913,7 +3775,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B70" s="5">
         <v>14.6</v>
@@ -3954,7 +3816,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="B71" s="5">
         <v>14.6</v>
@@ -3995,7 +3857,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B72" s="5">
         <v>14.6</v>
@@ -4036,7 +3898,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B73" s="5">
         <v>14.6</v>
@@ -4077,7 +3939,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="B74" s="5">
         <v>14.6</v>
@@ -4118,7 +3980,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B75" s="5">
         <v>14.6</v>
@@ -4159,7 +4021,7 @@
     </row>
     <row r="76" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B76" s="10">
         <v>14.6</v>

</xml_diff>

<commit_message>
restructuring of data science methods
</commit_message>
<xml_diff>
--- a/Data science methods/Exercise3_data.xlsx
+++ b/Data science methods/Exercise3_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\PycharmProjects\vu-gpa\Data science methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spapadokonstantakis\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C611D7D5-8F2C-4A48-88C5-E25417850CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36FF053-A3EB-45C4-AC3A-CD07ECA06512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C27C5E54-D3BB-418A-93AD-4D58CD294867}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C27C5E54-D3BB-418A-93AD-4D58CD294867}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,18 +41,53 @@
     <t>BD20 algae</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">BD20 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Camelina</t>
+    </r>
+  </si>
+  <si>
     <t>BD20 canola</t>
   </si>
   <si>
     <t>BD20 corn</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">BD20 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jatropha</t>
+    </r>
+  </si>
+  <si>
     <t>BD20 palm</t>
   </si>
   <si>
     <t>BD20 tallow</t>
   </si>
   <si>
+    <t>BD20 soy</t>
+  </si>
+  <si>
     <t>E10 corn A</t>
   </si>
   <si>
@@ -92,6 +127,38 @@
     <t>E10 grain sorghum</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">E10 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Miscanthus</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">E10 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Miscanthus*G</t>
+    </r>
+  </si>
+  <si>
     <t>E10 MSW</t>
   </si>
   <si>
@@ -161,6 +228,38 @@
     <t>E85 grain sorghum</t>
   </si>
   <si>
+    <r>
+      <t>E85</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Miscanthus</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>E85</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Miscanthus*G</t>
+    </r>
+  </si>
+  <si>
     <t>E85 MSW</t>
   </si>
   <si>
@@ -194,12 +293,44 @@
     <t>RDI algae</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">RDI </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Camelina</t>
+    </r>
+  </si>
+  <si>
     <t>RDI canola</t>
   </si>
   <si>
     <t>RDI corn</t>
   </si>
   <si>
+    <r>
+      <t>RDI </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jatropha</t>
+    </r>
+  </si>
+  <si>
     <t>RDI palm</t>
   </si>
   <si>
@@ -209,10 +340,42 @@
     <t>RDII algae</t>
   </si>
   <si>
+    <r>
+      <t>RDII </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Camelina</t>
+    </r>
+  </si>
+  <si>
     <t>RDII canola</t>
   </si>
   <si>
     <t>RDII corn</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RDII </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jatropha</t>
+    </r>
   </si>
   <si>
     <t>RDII palm</t>
@@ -499,45 +662,12 @@
       <t>kg 1,4-DCE]</t>
     </r>
   </si>
-  <si>
-    <t>BD20 Camelina</t>
-  </si>
-  <si>
-    <t>BD20 Jatropha</t>
-  </si>
-  <si>
-    <t>E10 Miscanthus</t>
-  </si>
-  <si>
-    <t>E10 Miscanthus*G</t>
-  </si>
-  <si>
-    <t>E85 Miscanthus</t>
-  </si>
-  <si>
-    <t>E85 Miscanthus*G</t>
-  </si>
-  <si>
-    <t>RDI Camelina</t>
-  </si>
-  <si>
-    <t>RDI Jatropha</t>
-  </si>
-  <si>
-    <t>RDII Camelina</t>
-  </si>
-  <si>
-    <t>RDII Jatropha</t>
-  </si>
-  <si>
-    <t>BD20 soy</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,6 +676,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -641,10 +779,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -656,16 +794,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -676,7 +814,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -692,9 +830,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -732,7 +870,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -838,7 +976,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -980,7 +1118,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -990,11 +1128,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122E9D76-EB91-4A73-B7B6-2ECBBBB4476A}">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="13" width="14" customWidth="1"/>
@@ -1003,79 +1141,79 @@
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="14" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1151,7 +1289,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="B6" s="5">
         <v>15.1</v>
@@ -1192,7 +1330,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="5">
         <v>15.1</v>
@@ -1233,7 +1371,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" s="5">
         <v>15.1</v>
@@ -1274,7 +1412,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="B9" s="5">
         <v>15.1</v>
@@ -1315,7 +1453,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10" s="5">
         <v>15.1</v>
@@ -1356,7 +1494,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" s="5">
         <v>15.1</v>
@@ -1397,7 +1535,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="B12" s="5">
         <v>15.1</v>
@@ -1438,7 +1576,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B13" s="5">
         <v>10.7</v>
@@ -1479,7 +1617,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B14" s="5">
         <v>10.7</v>
@@ -1520,7 +1658,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B15" s="5">
         <v>10.7</v>
@@ -1561,7 +1699,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B16" s="5">
         <v>10.7</v>
@@ -1602,7 +1740,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B17" s="5">
         <v>10.7</v>
@@ -1643,7 +1781,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B18" s="5">
         <v>10.7</v>
@@ -1684,7 +1822,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B19" s="5">
         <v>10.7</v>
@@ -1725,7 +1863,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B20" s="5">
         <v>10.7</v>
@@ -1766,7 +1904,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B21" s="5">
         <v>10.7</v>
@@ -1807,7 +1945,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B22" s="5">
         <v>10.7</v>
@@ -1848,7 +1986,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5">
         <v>10.7</v>
@@ -1889,7 +2027,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B24" s="5">
         <v>10.7</v>
@@ -1930,7 +2068,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B25" s="5">
         <v>10.7</v>
@@ -1971,7 +2109,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B26" s="5">
         <v>10.7</v>
@@ -2012,7 +2150,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="B27" s="5">
         <v>10.7</v>
@@ -2053,7 +2191,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B28" s="5">
         <v>10.7</v>
@@ -2094,7 +2232,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B29" s="5">
         <v>10.7</v>
@@ -2135,7 +2273,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B30" s="5">
         <v>10.7</v>
@@ -2176,7 +2314,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B31" s="5">
         <v>10.7</v>
@@ -2217,7 +2355,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B32" s="5">
         <v>10.7</v>
@@ -2258,7 +2396,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B33" s="5">
         <v>10.7</v>
@@ -2299,7 +2437,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B34" s="5">
         <v>10.7</v>
@@ -2340,7 +2478,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B35" s="5">
         <v>10.7</v>
@@ -2381,7 +2519,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B36" s="5">
         <v>10.7</v>
@@ -2422,7 +2560,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B37" s="7">
         <v>10.7</v>
@@ -2463,7 +2601,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B38" s="5">
         <v>8.6</v>
@@ -2504,7 +2642,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B39" s="5">
         <v>8.6</v>
@@ -2545,7 +2683,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B40" s="5">
         <v>8.6</v>
@@ -2586,7 +2724,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B41" s="5">
         <v>8.6</v>
@@ -2627,7 +2765,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B42" s="5">
         <v>8.6</v>
@@ -2668,7 +2806,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B43" s="5">
         <v>8.6</v>
@@ -2709,7 +2847,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B44" s="5">
         <v>8.6</v>
@@ -2750,7 +2888,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B45" s="5">
         <v>8.6</v>
@@ -2791,7 +2929,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B46" s="5">
         <v>8.6</v>
@@ -2832,7 +2970,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B47" s="5">
         <v>8.6</v>
@@ -2873,7 +3011,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B48" s="5">
         <v>8.6</v>
@@ -2914,7 +3052,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B49" s="5">
         <v>8.6</v>
@@ -2955,7 +3093,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B50" s="5">
         <v>8.6</v>
@@ -2996,7 +3134,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="B51" s="5">
         <v>8.6</v>
@@ -3037,7 +3175,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="B52" s="5">
         <v>8.6</v>
@@ -3078,7 +3216,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B53" s="5">
         <v>8.6</v>
@@ -3119,7 +3257,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B54" s="5">
         <v>8.6</v>
@@ -3160,7 +3298,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B55" s="5">
         <v>8.6</v>
@@ -3201,7 +3339,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B56" s="5">
         <v>8.6</v>
@@ -3242,7 +3380,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B57" s="5">
         <v>8.6</v>
@@ -3283,7 +3421,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B58" s="5">
         <v>8.6</v>
@@ -3324,7 +3462,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B59" s="5">
         <v>8.6</v>
@@ -3365,7 +3503,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B60" s="5">
         <v>8.6</v>
@@ -3406,7 +3544,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B61" s="5">
         <v>8.6</v>
@@ -3447,7 +3585,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B62" s="5">
         <v>8.6</v>
@@ -3488,7 +3626,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B63" s="5">
         <v>14.6</v>
@@ -3529,7 +3667,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="B64" s="5">
         <v>14.6</v>
@@ -3570,7 +3708,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B65" s="5">
         <v>14.6</v>
@@ -3611,7 +3749,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B66" s="5">
         <v>14.6</v>
@@ -3652,7 +3790,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="B67" s="5">
         <v>14.6</v>
@@ -3693,7 +3831,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B68" s="5">
         <v>14.6</v>
@@ -3734,7 +3872,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B69" s="5">
         <v>14.6</v>
@@ -3775,7 +3913,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B70" s="5">
         <v>14.6</v>
@@ -3816,7 +3954,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B71" s="5">
         <v>14.6</v>
@@ -3857,7 +3995,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B72" s="5">
         <v>14.6</v>
@@ -3898,7 +4036,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B73" s="5">
         <v>14.6</v>
@@ -3939,7 +4077,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B74" s="5">
         <v>14.6</v>
@@ -3980,7 +4118,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B75" s="5">
         <v>14.6</v>
@@ -4021,7 +4159,7 @@
     </row>
     <row r="76" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B76" s="10">
         <v>14.6</v>

</xml_diff>